<commit_message>
finalized fixes on the trenberth
</commit_message>
<xml_diff>
--- a/trenberth_figures/data/updated_trenberth_index.xlsx
+++ b/trenberth_figures/data/updated_trenberth_index.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P528"/>
+  <dimension ref="A1:P530"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -26782,6 +26782,106 @@
         <v>-34</v>
       </c>
     </row>
+    <row r="529">
+      <c r="A529" s="2" t="n">
+        <v>44896</v>
+      </c>
+      <c r="B529" t="n">
+        <v>-52</v>
+      </c>
+      <c r="C529" t="n">
+        <v>-29</v>
+      </c>
+      <c r="D529" t="n">
+        <v>-51</v>
+      </c>
+      <c r="E529" t="n">
+        <v>-52</v>
+      </c>
+      <c r="F529" t="n">
+        <v>-16</v>
+      </c>
+      <c r="G529" t="n">
+        <v>15</v>
+      </c>
+      <c r="H529" t="n">
+        <v>-8</v>
+      </c>
+      <c r="I529" t="n">
+        <v>23</v>
+      </c>
+      <c r="J529" t="n">
+        <v>-8</v>
+      </c>
+      <c r="K529" t="n">
+        <v>-31</v>
+      </c>
+      <c r="L529" t="n">
+        <v>-25</v>
+      </c>
+      <c r="M529" t="n">
+        <v>-10</v>
+      </c>
+      <c r="N529" t="n">
+        <v>-35</v>
+      </c>
+      <c r="O529" t="n">
+        <v>-16</v>
+      </c>
+      <c r="P529" t="n">
+        <v>-30</v>
+      </c>
+    </row>
+    <row r="530">
+      <c r="A530" s="2" t="n">
+        <v>44927</v>
+      </c>
+      <c r="B530" t="n">
+        <v>-102</v>
+      </c>
+      <c r="C530" t="n">
+        <v>-61</v>
+      </c>
+      <c r="D530" t="n">
+        <v>-92</v>
+      </c>
+      <c r="E530" t="n">
+        <v>-176</v>
+      </c>
+      <c r="F530" t="n">
+        <v>-49</v>
+      </c>
+      <c r="G530" t="n">
+        <v>-80</v>
+      </c>
+      <c r="H530" t="n">
+        <v>-95</v>
+      </c>
+      <c r="I530" t="n">
+        <v>14</v>
+      </c>
+      <c r="J530" t="n">
+        <v>13</v>
+      </c>
+      <c r="K530" t="n">
+        <v>-32</v>
+      </c>
+      <c r="L530" t="n">
+        <v>-116</v>
+      </c>
+      <c r="M530" t="n">
+        <v>-25</v>
+      </c>
+      <c r="N530" t="n">
+        <v>-79</v>
+      </c>
+      <c r="O530" t="n">
+        <v>-13</v>
+      </c>
+      <c r="P530" t="n">
+        <v>-80</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
fixed data issues with trenberth indices
</commit_message>
<xml_diff>
--- a/trenberth_figures/data/updated_trenberth_index.xlsx
+++ b/trenberth_figures/data/updated_trenberth_index.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P532"/>
+  <dimension ref="A1:P533"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -26526,41 +26526,101 @@
       <c r="A522" s="2" t="n">
         <v>44682</v>
       </c>
-      <c r="B522" t="inlineStr"/>
-      <c r="C522" t="inlineStr"/>
-      <c r="D522" t="inlineStr"/>
-      <c r="E522" t="inlineStr"/>
-      <c r="F522" t="inlineStr"/>
-      <c r="G522" t="inlineStr"/>
-      <c r="H522" t="inlineStr"/>
-      <c r="I522" t="inlineStr"/>
-      <c r="J522" t="inlineStr"/>
-      <c r="K522" t="inlineStr"/>
-      <c r="L522" t="inlineStr"/>
-      <c r="M522" t="inlineStr"/>
-      <c r="N522" t="inlineStr"/>
-      <c r="O522" t="inlineStr"/>
-      <c r="P522" t="inlineStr"/>
+      <c r="B522" t="n">
+        <v>13</v>
+      </c>
+      <c r="C522" t="n">
+        <v>22</v>
+      </c>
+      <c r="D522" t="n">
+        <v>19</v>
+      </c>
+      <c r="E522" t="n">
+        <v>-33</v>
+      </c>
+      <c r="F522" t="n">
+        <v>11</v>
+      </c>
+      <c r="G522" t="n">
+        <v>-60</v>
+      </c>
+      <c r="H522" t="n">
+        <v>-23</v>
+      </c>
+      <c r="I522" t="n">
+        <v>-38</v>
+      </c>
+      <c r="J522" t="n">
+        <v>9</v>
+      </c>
+      <c r="K522" t="n">
+        <v>21</v>
+      </c>
+      <c r="L522" t="n">
+        <v>-16</v>
+      </c>
+      <c r="M522" t="n">
+        <v>0</v>
+      </c>
+      <c r="N522" t="n">
+        <v>5</v>
+      </c>
+      <c r="O522" t="n">
+        <v>14</v>
+      </c>
+      <c r="P522" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="523">
       <c r="A523" s="2" t="n">
         <v>44713</v>
       </c>
-      <c r="B523" t="inlineStr"/>
-      <c r="C523" t="inlineStr"/>
-      <c r="D523" t="inlineStr"/>
-      <c r="E523" t="inlineStr"/>
-      <c r="F523" t="inlineStr"/>
-      <c r="G523" t="inlineStr"/>
-      <c r="H523" t="inlineStr"/>
-      <c r="I523" t="inlineStr"/>
-      <c r="J523" t="inlineStr"/>
-      <c r="K523" t="inlineStr"/>
-      <c r="L523" t="inlineStr"/>
-      <c r="M523" t="inlineStr"/>
-      <c r="N523" t="inlineStr"/>
-      <c r="O523" t="inlineStr"/>
-      <c r="P523" t="inlineStr"/>
+      <c r="B523" t="n">
+        <v>46</v>
+      </c>
+      <c r="C523" t="n">
+        <v>11</v>
+      </c>
+      <c r="D523" t="n">
+        <v>52</v>
+      </c>
+      <c r="E523" t="n">
+        <v>25</v>
+      </c>
+      <c r="F523" t="n">
+        <v>29</v>
+      </c>
+      <c r="G523" t="n">
+        <v>-8</v>
+      </c>
+      <c r="H523" t="n">
+        <v>-30</v>
+      </c>
+      <c r="I523" t="n">
+        <v>22</v>
+      </c>
+      <c r="J523" t="n">
+        <v>25</v>
+      </c>
+      <c r="K523" t="n">
+        <v>46</v>
+      </c>
+      <c r="L523" t="n">
+        <v>-7</v>
+      </c>
+      <c r="M523" t="n">
+        <v>8</v>
+      </c>
+      <c r="N523" t="n">
+        <v>23</v>
+      </c>
+      <c r="O523" t="n">
+        <v>29</v>
+      </c>
+      <c r="P523" t="n">
+        <v>-9</v>
+      </c>
     </row>
     <row r="524">
       <c r="A524" s="2" t="n">
@@ -26716,21 +26776,51 @@
       <c r="A527" s="2" t="n">
         <v>44835</v>
       </c>
-      <c r="B527" t="inlineStr"/>
-      <c r="C527" t="inlineStr"/>
-      <c r="D527" t="inlineStr"/>
-      <c r="E527" t="inlineStr"/>
-      <c r="F527" t="inlineStr"/>
-      <c r="G527" t="inlineStr"/>
-      <c r="H527" t="inlineStr"/>
-      <c r="I527" t="inlineStr"/>
-      <c r="J527" t="inlineStr"/>
-      <c r="K527" t="inlineStr"/>
-      <c r="L527" t="inlineStr"/>
-      <c r="M527" t="inlineStr"/>
-      <c r="N527" t="inlineStr"/>
-      <c r="O527" t="inlineStr"/>
-      <c r="P527" t="inlineStr"/>
+      <c r="B527" t="n">
+        <v>-24</v>
+      </c>
+      <c r="C527" t="n">
+        <v>14</v>
+      </c>
+      <c r="D527" t="n">
+        <v>-23</v>
+      </c>
+      <c r="E527" t="n">
+        <v>-44</v>
+      </c>
+      <c r="F527" t="n">
+        <v>-23</v>
+      </c>
+      <c r="G527" t="n">
+        <v>-21</v>
+      </c>
+      <c r="H527" t="n">
+        <v>7</v>
+      </c>
+      <c r="I527" t="n">
+        <v>-28</v>
+      </c>
+      <c r="J527" t="n">
+        <v>-10</v>
+      </c>
+      <c r="K527" t="n">
+        <v>-15</v>
+      </c>
+      <c r="L527" t="n">
+        <v>-3</v>
+      </c>
+      <c r="M527" t="n">
+        <v>-9</v>
+      </c>
+      <c r="N527" t="n">
+        <v>-21</v>
+      </c>
+      <c r="O527" t="n">
+        <v>-3</v>
+      </c>
+      <c r="P527" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="528">
       <c r="A528" s="2" t="n">
@@ -26937,49 +27027,99 @@
         <v>44986</v>
       </c>
       <c r="B532" t="n">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="C532" t="n">
-        <v>-20</v>
+        <v>-4</v>
       </c>
       <c r="D532" t="n">
+        <v>20</v>
+      </c>
+      <c r="E532" t="n">
+        <v>59</v>
+      </c>
+      <c r="F532" t="n">
         <v>15</v>
       </c>
-      <c r="E532" t="n">
-        <v>27</v>
-      </c>
-      <c r="F532" t="n">
-        <v>54</v>
-      </c>
       <c r="G532" t="n">
-        <v>-58</v>
+        <v>5</v>
       </c>
       <c r="H532" t="n">
-        <v>13</v>
+        <v>34</v>
       </c>
       <c r="I532" t="n">
-        <v>-72</v>
+        <v>-30</v>
       </c>
       <c r="J532" t="n">
-        <v>-6</v>
+        <v>-5</v>
       </c>
       <c r="K532" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="L532" t="n">
-        <v>17</v>
+        <v>42</v>
       </c>
       <c r="M532" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="N532" t="n">
+        <v>18</v>
+      </c>
+      <c r="O532" t="n">
+        <v>1</v>
+      </c>
+      <c r="P532" t="n">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="533">
+      <c r="A533" s="2" t="n">
+        <v>45017</v>
+      </c>
+      <c r="B533" t="n">
+        <v>-4</v>
+      </c>
+      <c r="C533" t="n">
+        <v>-37</v>
+      </c>
+      <c r="D533" t="n">
+        <v>4</v>
+      </c>
+      <c r="E533" t="n">
+        <v>-1</v>
+      </c>
+      <c r="F533" t="n">
+        <v>-13</v>
+      </c>
+      <c r="G533" t="n">
         <v>7</v>
       </c>
-      <c r="O532" t="n">
-        <v>8</v>
-      </c>
-      <c r="P532" t="n">
-        <v>-41</v>
+      <c r="H533" t="n">
+        <v>-31</v>
+      </c>
+      <c r="I533" t="n">
+        <v>38</v>
+      </c>
+      <c r="J533" t="n">
+        <v>5</v>
+      </c>
+      <c r="K533" t="n">
+        <v>7</v>
+      </c>
+      <c r="L533" t="n">
+        <v>-29</v>
+      </c>
+      <c r="M533" t="n">
+        <v>-1</v>
+      </c>
+      <c r="N533" t="n">
+        <v>-10</v>
+      </c>
+      <c r="O533" t="n">
+        <v>14</v>
+      </c>
+      <c r="P533" t="n">
+        <v>-54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>